<commit_message>
tdf#40517 Unit test for question marks in number format
Unit test for https://gerrit.libreoffice.org/21021/

Change-Id: I958ccdcc68a4e496cbd4bdc74d0650c133f3a3f7
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/universal-content.xlsx
+++ b/sc/qa/unit/data/xlsx/universal-content.xlsx
@@ -2,57 +2,42 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="141" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:v2="http://schemas.openxmlformats.org/spreadsheetml/2006/main/v2" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="v2">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="H3">
+    <comment ref="H3" authorId="0">
       <text>
         <r>
           <rPr>
+            <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <sz val="10"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Test</t>
+          <t>Test</t>
         </r>
       </text>
-      <mc:AlternateContent>
-        <mc:Choice Requires="v2">
-          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
-            <anchor moveWithCells="false" sizeWithCells="false">
-              <xdr:from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </xdr:from>
-              <xdr:to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>47</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>6</xdr:rowOff>
-              </xdr:to>
-            </anchor>
-          </commentPr>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
     </comment>
   </commentList>
 </comments>
@@ -61,39 +46,41 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>String1</t>
+    <t xml:space="preserve">String1</t>
   </si>
   <si>
-    <t>String2</t>
+    <t xml:space="preserve">String2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.???"/>
   </numFmts>
   <fonts count="4">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,7 +92,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -114,40 +101,51 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -157,18 +155,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H3" activeCellId="0" pane="topLeft" sqref="H3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="n">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -179,7 +178,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="10.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
@@ -190,14 +189,18 @@
         <f aca="false">2+3</f>
         <v>5</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="3">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="10.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="n">
         <f aca="false">2-3</f>
         <v>-1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="10.55" outlineLevel="0" r="4">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="10.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="n">
         <f aca="false">C1+C2</f>
         <v>11</v>
@@ -209,7 +212,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -225,17 +228,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>